<commit_message>
Modify the point of pointed out. https://github.com/OpenTouryoProject/OpenTouryoDocuments/pull/20
</commit_message>
<xml_diff>
--- a/documents/0_Introduction/ja-JP/Functional_list.xlsx
+++ b/documents/0_Introduction/ja-JP/Functional_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="21420" windowHeight="10575" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="21420" windowHeight="10575"/>
   </bookViews>
   <sheets>
     <sheet name="参考" sheetId="8" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="321">
   <si>
     <t>（その他、ベース２カスタマイズで追加可能）</t>
     <rPh sb="3" eb="4">
@@ -906,22 +906,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>・スニペット＆テンプレート</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・コード スニペット</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・項目テンプレート</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>・プロジェクト テンプレート</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>・Windows Forms用P層フレームワーク テスト</t>
     <rPh sb="14" eb="15">
       <t>ヨウ</t>
@@ -1016,10 +1000,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>○</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>・Silverlight（CRUD）</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1236,14 +1216,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>上記に習って追加可能</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>上記に習って追加可能</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>バッチ</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1780,14 +1752,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>SPA等の
-クライアント</t>
-    <rPh sb="3" eb="4">
-      <t>ナド</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ASP.NET
 MVC</t>
     <phoneticPr fontId="1"/>
@@ -1832,6 +1796,25 @@
   </si>
   <si>
     <t>Releases · OpenTouryoProject/OpenTouryoTemplates</t>
+  </si>
+  <si>
+    <t>SPA
+(Single Page Application)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>上記に倣って追加可能</t>
+    <rPh sb="3" eb="4">
+      <t>ナラ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>上記に倣って追加可能</t>
+    <rPh sb="3" eb="4">
+      <t>ナラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -2103,7 +2086,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2362,58 +2345,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2457,6 +2392,63 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2765,38 +2757,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B3" s="117" t="s">
-        <v>324</v>
+      <c r="B3" s="101" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B6" s="117" t="s">
-        <v>323</v>
+      <c r="B6" s="101" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C8" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C9" s="117" t="s">
-        <v>322</v>
+      <c r="C9" s="101" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2828,38 +2820,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="86" t="s">
+      <c r="C1" s="104"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="89" t="s">
-        <v>208</v>
-      </c>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="91"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="106" t="s">
+        <v>203</v>
+      </c>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="108"/>
       <c r="U1" s="71"/>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A2" s="85"/>
+      <c r="A2" s="102"/>
       <c r="B2" s="4" t="s">
         <v>34</v>
       </c>
@@ -2872,21 +2864,21 @@
       <c r="E2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="F2" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
       <c r="N2" s="53" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="O2" s="54" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>67</v>
@@ -2895,13 +2887,13 @@
         <v>68</v>
       </c>
       <c r="R2" s="56" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="S2" s="75" t="s">
-        <v>313</v>
-      </c>
-      <c r="T2" s="105" t="s">
-        <v>314</v>
+        <v>306</v>
+      </c>
+      <c r="T2" s="89" t="s">
+        <v>318</v>
       </c>
       <c r="U2" s="71"/>
     </row>
@@ -2978,7 +2970,7 @@
       <c r="B5" s="5"/>
       <c r="C5" s="10"/>
       <c r="E5" s="7" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -3017,7 +3009,7 @@
       <c r="B6" s="5"/>
       <c r="C6" s="10"/>
       <c r="E6" s="7" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -3056,7 +3048,7 @@
       <c r="B7" s="5"/>
       <c r="C7" s="10"/>
       <c r="E7" s="7" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -3095,7 +3087,7 @@
       <c r="B8" s="5"/>
       <c r="C8" s="11"/>
       <c r="E8" s="15" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -3198,7 +3190,7 @@
         <v>38</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="S10" s="3" t="s">
         <v>132</v>
@@ -3415,7 +3407,7 @@
       <c r="C16" s="20"/>
       <c r="D16" s="29"/>
       <c r="E16" s="15" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="17"/>
@@ -3426,10 +3418,10 @@
       <c r="L16" s="8"/>
       <c r="M16" s="9"/>
       <c r="N16" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="P16" s="3" t="s">
         <v>38</v>
@@ -3438,13 +3430,13 @@
         <v>38</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.15">
@@ -3455,7 +3447,7 @@
       <c r="C17" s="20"/>
       <c r="D17" s="29"/>
       <c r="E17" s="15" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="17"/>
@@ -3469,7 +3461,7 @@
         <v>38</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>38</v>
@@ -3666,16 +3658,16 @@
       <c r="L22" s="8"/>
       <c r="M22" s="9"/>
       <c r="N22" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="R22" s="3" t="s">
         <v>38</v>
@@ -3695,7 +3687,7 @@
       <c r="C23" s="20"/>
       <c r="D23" s="22"/>
       <c r="E23" s="15" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="17"/>
@@ -3709,10 +3701,10 @@
         <v>38</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>38</v>
@@ -3735,7 +3727,7 @@
       <c r="C24" s="20"/>
       <c r="D24" s="70"/>
       <c r="E24" s="15" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="17"/>
@@ -3746,10 +3738,10 @@
       <c r="L24" s="8"/>
       <c r="M24" s="9"/>
       <c r="N24" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="P24" s="3" t="s">
         <v>119</v>
@@ -3758,13 +3750,13 @@
         <v>119</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.15">
@@ -3773,7 +3765,7 @@
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="8"/>
@@ -3935,7 +3927,7 @@
       <c r="C29" s="20"/>
       <c r="D29" s="26"/>
       <c r="E29" s="24" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
@@ -4013,7 +4005,7 @@
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="7" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D31" s="14"/>
       <c r="E31" s="8"/>
@@ -4055,7 +4047,7 @@
       <c r="C32" s="20"/>
       <c r="D32" s="26"/>
       <c r="E32" s="15" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="17"/>
@@ -4095,7 +4087,7 @@
       <c r="C33" s="20"/>
       <c r="D33" s="26"/>
       <c r="E33" s="15" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="17"/>
@@ -4149,7 +4141,7 @@
         <v>38</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P34" s="3" t="s">
         <v>38</v>
@@ -4175,7 +4167,7 @@
       <c r="C35" s="20"/>
       <c r="D35" s="26"/>
       <c r="E35" s="15" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
@@ -4215,7 +4207,7 @@
       <c r="C36" s="20"/>
       <c r="D36" s="26"/>
       <c r="E36" s="15" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
@@ -4255,7 +4247,7 @@
       <c r="C37" s="20"/>
       <c r="D37" s="26"/>
       <c r="E37" s="15" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
@@ -4287,7 +4279,7 @@
         <v>132</v>
       </c>
       <c r="U37" s="73" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.15">
@@ -4298,7 +4290,7 @@
       <c r="C38" s="20"/>
       <c r="D38" s="26"/>
       <c r="E38" s="15" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
@@ -4354,7 +4346,7 @@
         <v>38</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P39" s="3" t="s">
         <v>38</v>
@@ -4378,7 +4370,7 @@
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="7" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D40" s="14"/>
       <c r="E40" s="8"/>
@@ -4460,7 +4452,7 @@
       <c r="C42" s="20"/>
       <c r="D42" s="29"/>
       <c r="E42" s="15" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="17"/>
@@ -4500,7 +4492,7 @@
       <c r="C43" s="21"/>
       <c r="D43" s="30"/>
       <c r="E43" s="15" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="17"/>
@@ -4534,10 +4526,10 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.15">
       <c r="E45" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="N45" s="68" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.15">
@@ -4545,10 +4537,10 @@
         <v>119</v>
       </c>
       <c r="F46" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="N46" s="68" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.15">
@@ -4556,18 +4548,18 @@
         <v>38</v>
       </c>
       <c r="F47" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="N47" s="68" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.15">
       <c r="E48" s="37" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F48" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.15">
@@ -4583,15 +4575,15 @@
         <v>139</v>
       </c>
       <c r="F50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="5:6" x14ac:dyDescent="0.15">
       <c r="E51" s="66" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F51" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -4625,37 +4617,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="86" t="s">
+      <c r="C1" s="104"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="85" t="s">
-        <v>208</v>
-      </c>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="102" t="s">
+        <v>203</v>
+      </c>
+      <c r="O1" s="102"/>
+      <c r="P1" s="102"/>
+      <c r="Q1" s="102"/>
+      <c r="R1" s="102"/>
+      <c r="S1" s="102"/>
+      <c r="T1" s="102"/>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A2" s="85"/>
+      <c r="A2" s="102"/>
       <c r="B2" s="4" t="s">
         <v>34</v>
       </c>
@@ -4668,21 +4660,21 @@
       <c r="E2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="F2" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
       <c r="N2" s="53" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="O2" s="54" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>67</v>
@@ -4691,13 +4683,13 @@
         <v>68</v>
       </c>
       <c r="R2" s="56" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="S2" s="75" t="s">
-        <v>313</v>
-      </c>
-      <c r="T2" s="105" t="s">
-        <v>314</v>
+        <v>306</v>
+      </c>
+      <c r="T2" s="89" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.15">
@@ -4846,7 +4838,7 @@
         <v>132</v>
       </c>
       <c r="U6" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.15">
@@ -4889,7 +4881,7 @@
         <v>132</v>
       </c>
       <c r="U7" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.15">
@@ -4932,7 +4924,7 @@
         <v>132</v>
       </c>
       <c r="U8" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.15">
@@ -5095,7 +5087,7 @@
         <v>39</v>
       </c>
       <c r="U12" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.15">
@@ -5138,7 +5130,7 @@
         <v>39</v>
       </c>
       <c r="U13" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.15">
@@ -5181,7 +5173,7 @@
         <v>39</v>
       </c>
       <c r="U14" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.15">
@@ -5272,7 +5264,7 @@
         <v>38</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>38</v>
@@ -5312,7 +5304,7 @@
         <v>38</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>38</v>
@@ -5352,7 +5344,7 @@
         <v>38</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>38</v>
@@ -5370,7 +5362,7 @@
         <v>132</v>
       </c>
       <c r="U19" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.15">
@@ -5395,7 +5387,7 @@
         <v>38</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P20" s="3" t="s">
         <v>38</v>
@@ -5413,7 +5405,7 @@
         <v>132</v>
       </c>
       <c r="U20" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.15">
@@ -5424,7 +5416,7 @@
       <c r="C21" s="10"/>
       <c r="D21" s="19"/>
       <c r="E21" s="7" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="25"/>
@@ -5438,7 +5430,7 @@
         <v>38</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>38</v>
@@ -5464,7 +5456,7 @@
       <c r="C22" s="10"/>
       <c r="D22" s="19"/>
       <c r="E22" s="7" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="25"/>
@@ -5478,7 +5470,7 @@
         <v>38</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P22" s="3" t="s">
         <v>38</v>
@@ -5502,7 +5494,7 @@
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="7" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="8"/>
@@ -5518,7 +5510,7 @@
         <v>38</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P23" s="3" t="s">
         <v>38</v>
@@ -5544,7 +5536,7 @@
       <c r="C24" s="10"/>
       <c r="D24" s="19"/>
       <c r="E24" s="15" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="17"/>
@@ -5555,13 +5547,13 @@
       <c r="L24" s="8"/>
       <c r="M24" s="9"/>
       <c r="N24" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>132</v>
@@ -5584,7 +5576,7 @@
       <c r="C25" s="10"/>
       <c r="D25" s="19"/>
       <c r="E25" s="15" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="17"/>
@@ -5595,13 +5587,13 @@
       <c r="L25" s="8"/>
       <c r="M25" s="9"/>
       <c r="N25" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>132</v>
@@ -5624,7 +5616,7 @@
       <c r="C26" s="10"/>
       <c r="D26" s="19"/>
       <c r="E26" s="15" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="17"/>
@@ -5635,13 +5627,13 @@
       <c r="L26" s="8"/>
       <c r="M26" s="9"/>
       <c r="N26" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="Q26" s="3" t="s">
         <v>132</v>
@@ -5678,7 +5670,7 @@
         <v>38</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P27" s="3" t="s">
         <v>38</v>
@@ -5718,7 +5710,7 @@
         <v>38</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P28" s="3" t="s">
         <v>38</v>
@@ -5758,7 +5750,7 @@
         <v>38</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="P29" s="3" t="s">
         <v>38</v>
@@ -5784,7 +5776,7 @@
       <c r="C30" s="20"/>
       <c r="D30" s="29"/>
       <c r="E30" s="15" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="17"/>
@@ -5824,7 +5816,7 @@
       <c r="C31" s="20"/>
       <c r="D31" s="29"/>
       <c r="E31" s="15" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="17"/>
@@ -5838,7 +5830,7 @@
         <v>38</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P31" s="3" t="s">
         <v>38</v>
@@ -5891,7 +5883,7 @@
       <c r="D33" s="29"/>
       <c r="E33" s="5"/>
       <c r="F33" s="8" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="G33" s="17"/>
       <c r="H33" s="8"/>
@@ -5904,7 +5896,7 @@
         <v>38</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P33" s="3" t="s">
         <v>38</v>
@@ -5940,25 +5932,25 @@
       <c r="K34" s="14"/>
       <c r="L34" s="14"/>
       <c r="M34" s="50"/>
-      <c r="N34" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="O34" s="92" t="s">
-        <v>180</v>
+      <c r="N34" s="109" t="s">
+        <v>38</v>
+      </c>
+      <c r="O34" s="109" t="s">
+        <v>176</v>
       </c>
       <c r="P34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Q34" s="92" t="s">
+      <c r="Q34" s="109" t="s">
         <v>132</v>
       </c>
       <c r="R34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S34" s="92" t="s">
-        <v>132</v>
-      </c>
-      <c r="T34" s="92" t="s">
+      <c r="S34" s="109" t="s">
+        <v>132</v>
+      </c>
+      <c r="T34" s="109" t="s">
         <v>132</v>
       </c>
     </row>
@@ -5971,7 +5963,7 @@
       <c r="D35" s="29"/>
       <c r="E35" s="77"/>
       <c r="F35" s="16" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="G35" s="23"/>
       <c r="H35" s="16"/>
@@ -5980,17 +5972,17 @@
       <c r="K35" s="16"/>
       <c r="L35" s="16"/>
       <c r="M35" s="13"/>
-      <c r="N35" s="97"/>
-      <c r="O35" s="97"/>
+      <c r="N35" s="110"/>
+      <c r="O35" s="110"/>
       <c r="P35" s="55" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q35" s="97"/>
+        <v>193</v>
+      </c>
+      <c r="Q35" s="110"/>
       <c r="R35" s="55" t="s">
-        <v>198</v>
-      </c>
-      <c r="S35" s="93"/>
-      <c r="T35" s="93"/>
+        <v>193</v>
+      </c>
+      <c r="S35" s="111"/>
+      <c r="T35" s="111"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A36" s="76">
@@ -6014,7 +6006,7 @@
         <v>38</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P36" s="3" t="s">
         <v>38</v>
@@ -6054,7 +6046,7 @@
         <v>38</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P37" s="3" t="s">
         <v>38</v>
@@ -6094,7 +6086,7 @@
         <v>38</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P38" s="3" t="s">
         <v>38</v>
@@ -6134,7 +6126,7 @@
         <v>38</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P39" s="3" t="s">
         <v>38</v>
@@ -6174,7 +6166,7 @@
         <v>38</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P40" s="3" t="s">
         <v>38</v>
@@ -6214,7 +6206,7 @@
         <v>38</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P41" s="3" t="s">
         <v>38</v>
@@ -6254,7 +6246,7 @@
         <v>38</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P42" s="3" t="s">
         <v>38</v>
@@ -6294,7 +6286,7 @@
         <v>38</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P43" s="3" t="s">
         <v>38</v>
@@ -6334,7 +6326,7 @@
         <v>38</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P44" s="3" t="s">
         <v>38</v>
@@ -6360,16 +6352,16 @@
       <c r="C45" s="20"/>
       <c r="D45" s="29"/>
       <c r="E45" s="5"/>
-      <c r="F45" s="113" t="s">
-        <v>319</v>
-      </c>
-      <c r="G45" s="114"/>
-      <c r="H45" s="115"/>
-      <c r="I45" s="115"/>
-      <c r="J45" s="115"/>
-      <c r="K45" s="115"/>
-      <c r="L45" s="115"/>
-      <c r="M45" s="116"/>
+      <c r="F45" s="97" t="s">
+        <v>311</v>
+      </c>
+      <c r="G45" s="98"/>
+      <c r="H45" s="99"/>
+      <c r="I45" s="99"/>
+      <c r="J45" s="99"/>
+      <c r="K45" s="99"/>
+      <c r="L45" s="99"/>
+      <c r="M45" s="100"/>
       <c r="N45" s="3" t="s">
         <v>38</v>
       </c>
@@ -6401,7 +6393,7 @@
       <c r="D46" s="30"/>
       <c r="E46" s="6"/>
       <c r="F46" s="15" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G46" s="17"/>
       <c r="H46" s="8"/>
@@ -6410,25 +6402,25 @@
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="M46" s="9"/>
-      <c r="N46" s="94" t="s">
-        <v>224</v>
-      </c>
-      <c r="O46" s="95"/>
-      <c r="P46" s="95"/>
-      <c r="Q46" s="95"/>
-      <c r="R46" s="95"/>
-      <c r="S46" s="95"/>
-      <c r="T46" s="96"/>
+      <c r="N46" s="112" t="s">
+        <v>320</v>
+      </c>
+      <c r="O46" s="113"/>
+      <c r="P46" s="113"/>
+      <c r="Q46" s="113"/>
+      <c r="R46" s="113"/>
+      <c r="S46" s="113"/>
+      <c r="T46" s="114"/>
       <c r="U46" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.15">
       <c r="E48" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="N48" s="67" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="5:14" x14ac:dyDescent="0.15">
@@ -6436,10 +6428,10 @@
         <v>119</v>
       </c>
       <c r="F49" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="N49" s="67" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="5:14" x14ac:dyDescent="0.15">
@@ -6447,21 +6439,21 @@
         <v>38</v>
       </c>
       <c r="F50" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="N50" s="67" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="51" spans="5:14" x14ac:dyDescent="0.15">
       <c r="E51" s="37" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F51" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="N51" s="67" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" spans="5:14" x14ac:dyDescent="0.15">
@@ -6477,30 +6469,30 @@
         <v>139</v>
       </c>
       <c r="F53" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="5:14" x14ac:dyDescent="0.15">
       <c r="E54" s="66" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F54" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T34:T35"/>
+    <mergeCell ref="S34:S35"/>
+    <mergeCell ref="N46:T46"/>
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="O34:O35"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:M1"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="Q34:Q35"/>
     <mergeCell ref="N34:N35"/>
-    <mergeCell ref="T34:T35"/>
-    <mergeCell ref="S34:S35"/>
-    <mergeCell ref="N46:T46"/>
-    <mergeCell ref="N1:T1"/>
-    <mergeCell ref="O34:O35"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -6528,37 +6520,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="86" t="s">
+      <c r="C1" s="104"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="86" t="s">
-        <v>228</v>
-      </c>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="88"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="103" t="s">
+        <v>221</v>
+      </c>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="104"/>
+      <c r="R1" s="104"/>
+      <c r="S1" s="104"/>
+      <c r="T1" s="105"/>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A2" s="85"/>
+      <c r="A2" s="102"/>
       <c r="B2" s="4" t="s">
         <v>34</v>
       </c>
@@ -6571,24 +6563,24 @@
       <c r="E2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="F2" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="88"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="105"/>
       <c r="N2" s="75" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="O2" s="75" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="P2" s="65" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="Q2" s="33" t="s">
         <v>126</v>
@@ -6597,10 +6589,10 @@
         <v>37</v>
       </c>
       <c r="S2" s="75" t="s">
-        <v>313</v>
-      </c>
-      <c r="T2" s="105" t="s">
-        <v>314</v>
+        <v>306</v>
+      </c>
+      <c r="T2" s="89" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.15">
@@ -6677,7 +6669,7 @@
       <c r="C5" s="10"/>
       <c r="D5" s="12"/>
       <c r="E5" s="7" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -6749,7 +6741,7 @@
         <v>39</v>
       </c>
       <c r="U6" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.15">
@@ -7082,7 +7074,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="15" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -7122,7 +7114,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="7" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -7162,7 +7154,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="7" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -7202,7 +7194,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="7" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -7250,25 +7242,25 @@
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
       <c r="M19" s="50"/>
-      <c r="N19" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="O19" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="P19" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q19" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="R19" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="S19" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="T19" s="92" t="s">
+      <c r="N19" s="109" t="s">
+        <v>38</v>
+      </c>
+      <c r="O19" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="P19" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q19" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="R19" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="S19" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="T19" s="109" t="s">
         <v>39</v>
       </c>
     </row>
@@ -7290,13 +7282,13 @@
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
       <c r="M20" s="13"/>
-      <c r="N20" s="93"/>
-      <c r="O20" s="93"/>
-      <c r="P20" s="93"/>
-      <c r="Q20" s="93"/>
-      <c r="R20" s="93"/>
-      <c r="S20" s="93"/>
-      <c r="T20" s="93"/>
+      <c r="N20" s="111"/>
+      <c r="O20" s="111"/>
+      <c r="P20" s="111"/>
+      <c r="Q20" s="111"/>
+      <c r="R20" s="111"/>
+      <c r="S20" s="111"/>
+      <c r="T20" s="111"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A21" s="76">
@@ -7378,7 +7370,7 @@
         <v>39</v>
       </c>
       <c r="U22" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.15">
@@ -7421,7 +7413,7 @@
         <v>39</v>
       </c>
       <c r="U23" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.15">
@@ -7845,7 +7837,7 @@
       <c r="N34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O34" s="106" t="s">
+      <c r="O34" s="90" t="s">
         <v>38</v>
       </c>
       <c r="P34" s="3" t="s">
@@ -7885,7 +7877,7 @@
       <c r="N35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O35" s="106" t="s">
+      <c r="O35" s="90" t="s">
         <v>38</v>
       </c>
       <c r="P35" s="3" t="s">
@@ -7925,7 +7917,7 @@
       <c r="N36" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O36" s="106" t="s">
+      <c r="O36" s="90" t="s">
         <v>38</v>
       </c>
       <c r="P36" s="3" t="s">
@@ -8365,7 +8357,7 @@
       <c r="N47" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O47" s="106" t="s">
+      <c r="O47" s="90" t="s">
         <v>38</v>
       </c>
       <c r="P47" s="3" t="s">
@@ -8393,7 +8385,7 @@
       <c r="D48" s="12"/>
       <c r="E48" s="10"/>
       <c r="F48" s="21" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
@@ -8403,10 +8395,10 @@
       <c r="L48" s="8"/>
       <c r="M48" s="9"/>
       <c r="N48" s="3" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="P48" s="3" t="s">
         <v>39</v>
@@ -8424,7 +8416,7 @@
         <v>39</v>
       </c>
       <c r="U48" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.15">
@@ -8528,7 +8520,7 @@
       <c r="N51" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O51" s="106" t="s">
+      <c r="O51" s="90" t="s">
         <v>38</v>
       </c>
       <c r="P51" s="3" t="s">
@@ -8568,7 +8560,7 @@
       <c r="N52" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O52" s="106" t="s">
+      <c r="O52" s="90" t="s">
         <v>38</v>
       </c>
       <c r="P52" s="3" t="s">
@@ -8781,7 +8773,7 @@
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="7" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
@@ -8853,7 +8845,7 @@
         <v>39</v>
       </c>
       <c r="U59" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.15">
@@ -9336,7 +9328,7 @@
         <v>39</v>
       </c>
       <c r="U71" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.15">
@@ -9379,7 +9371,7 @@
         <v>39</v>
       </c>
       <c r="U72" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.15">
@@ -9639,7 +9631,7 @@
       <c r="J79" s="27"/>
       <c r="K79" s="27"/>
       <c r="L79" s="27"/>
-      <c r="M79" s="104"/>
+      <c r="M79" s="88"/>
       <c r="N79" s="28" t="s">
         <v>39</v>
       </c>
@@ -9653,7 +9645,7 @@
         <v>39</v>
       </c>
       <c r="R79" s="28" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="S79" s="28" t="s">
         <v>39</v>
@@ -9670,7 +9662,7 @@
       <c r="C80" s="5"/>
       <c r="D80" s="32"/>
       <c r="E80" s="15" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F80" s="27"/>
       <c r="G80" s="27"/>
@@ -9679,7 +9671,7 @@
       <c r="J80" s="27"/>
       <c r="K80" s="27"/>
       <c r="L80" s="27"/>
-      <c r="M80" s="104"/>
+      <c r="M80" s="88"/>
       <c r="N80" s="28" t="s">
         <v>39</v>
       </c>
@@ -9693,7 +9685,7 @@
         <v>39</v>
       </c>
       <c r="R80" s="28" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="S80" s="28" t="s">
         <v>39</v>
@@ -9719,7 +9711,7 @@
       <c r="J81" s="27"/>
       <c r="K81" s="27"/>
       <c r="L81" s="27"/>
-      <c r="M81" s="104"/>
+      <c r="M81" s="88"/>
       <c r="N81" s="28" t="s">
         <v>39</v>
       </c>
@@ -9733,7 +9725,7 @@
         <v>39</v>
       </c>
       <c r="R81" s="28" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="S81" s="28" t="s">
         <v>39</v>
@@ -9750,7 +9742,7 @@
       <c r="C82" s="5"/>
       <c r="D82" s="81"/>
       <c r="E82" s="15" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F82" s="27"/>
       <c r="G82" s="27"/>
@@ -9759,7 +9751,7 @@
       <c r="J82" s="27"/>
       <c r="K82" s="27"/>
       <c r="L82" s="27"/>
-      <c r="M82" s="104"/>
+      <c r="M82" s="88"/>
       <c r="N82" s="28" t="s">
         <v>39</v>
       </c>
@@ -9773,7 +9765,7 @@
         <v>39</v>
       </c>
       <c r="R82" s="28" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="S82" s="28" t="s">
         <v>39</v>
@@ -9788,7 +9780,7 @@
       </c>
       <c r="B83" s="10"/>
       <c r="C83" s="7" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E83" s="8"/>
       <c r="F83" s="8"/>
@@ -9807,7 +9799,7 @@
       <c r="S83" s="40"/>
       <c r="T83" s="41"/>
       <c r="U83" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="84" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -9817,7 +9809,7 @@
       <c r="B84" s="10"/>
       <c r="C84" s="20"/>
       <c r="D84" s="44" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E84" s="49"/>
       <c r="F84" s="49"/>
@@ -9850,7 +9842,7 @@
         <v>142</v>
       </c>
       <c r="U84" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="85" spans="1:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.15">
@@ -9860,17 +9852,17 @@
       <c r="B85" s="10"/>
       <c r="C85" s="20"/>
       <c r="D85" s="22"/>
-      <c r="E85" s="98" t="s">
-        <v>285</v>
-      </c>
-      <c r="F85" s="98"/>
-      <c r="G85" s="98"/>
-      <c r="H85" s="98"/>
-      <c r="I85" s="98"/>
-      <c r="J85" s="98"/>
-      <c r="K85" s="98"/>
-      <c r="L85" s="98"/>
-      <c r="M85" s="98"/>
+      <c r="E85" s="115" t="s">
+        <v>278</v>
+      </c>
+      <c r="F85" s="115"/>
+      <c r="G85" s="115"/>
+      <c r="H85" s="115"/>
+      <c r="I85" s="115"/>
+      <c r="J85" s="115"/>
+      <c r="K85" s="115"/>
+      <c r="L85" s="115"/>
+      <c r="M85" s="115"/>
       <c r="N85" s="3" t="s">
         <v>142</v>
       </c>
@@ -9893,7 +9885,7 @@
         <v>142</v>
       </c>
       <c r="U85" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="86" spans="1:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.15">
@@ -9903,17 +9895,17 @@
       <c r="B86" s="10"/>
       <c r="C86" s="22"/>
       <c r="D86" s="22"/>
-      <c r="E86" s="98" t="s">
-        <v>264</v>
-      </c>
-      <c r="F86" s="98"/>
-      <c r="G86" s="98"/>
-      <c r="H86" s="98"/>
-      <c r="I86" s="98"/>
-      <c r="J86" s="98"/>
-      <c r="K86" s="98"/>
-      <c r="L86" s="98"/>
-      <c r="M86" s="98"/>
+      <c r="E86" s="115" t="s">
+        <v>257</v>
+      </c>
+      <c r="F86" s="115"/>
+      <c r="G86" s="115"/>
+      <c r="H86" s="115"/>
+      <c r="I86" s="115"/>
+      <c r="J86" s="115"/>
+      <c r="K86" s="115"/>
+      <c r="L86" s="115"/>
+      <c r="M86" s="115"/>
       <c r="N86" s="3" t="s">
         <v>142</v>
       </c>
@@ -9936,7 +9928,7 @@
         <v>142</v>
       </c>
       <c r="U86" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="87" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -9946,7 +9938,7 @@
       <c r="B87" s="10"/>
       <c r="C87" s="22"/>
       <c r="D87" s="44" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E87" s="49"/>
       <c r="F87" s="49"/>
@@ -9979,7 +9971,7 @@
         <v>142</v>
       </c>
       <c r="U87" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="88" spans="1:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.15">
@@ -9989,17 +9981,17 @@
       <c r="B88" s="10"/>
       <c r="C88" s="22"/>
       <c r="D88" s="22"/>
-      <c r="E88" s="99" t="s">
-        <v>285</v>
-      </c>
-      <c r="F88" s="100"/>
-      <c r="G88" s="100"/>
-      <c r="H88" s="100"/>
-      <c r="I88" s="100"/>
-      <c r="J88" s="100"/>
-      <c r="K88" s="100"/>
-      <c r="L88" s="100"/>
-      <c r="M88" s="101"/>
+      <c r="E88" s="116" t="s">
+        <v>278</v>
+      </c>
+      <c r="F88" s="117"/>
+      <c r="G88" s="117"/>
+      <c r="H88" s="117"/>
+      <c r="I88" s="117"/>
+      <c r="J88" s="117"/>
+      <c r="K88" s="117"/>
+      <c r="L88" s="117"/>
+      <c r="M88" s="118"/>
       <c r="N88" s="3" t="s">
         <v>38</v>
       </c>
@@ -10022,7 +10014,7 @@
         <v>142</v>
       </c>
       <c r="U88" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="89" spans="1:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.15">
@@ -10032,17 +10024,17 @@
       <c r="B89" s="10"/>
       <c r="C89" s="77"/>
       <c r="D89" s="77"/>
-      <c r="E89" s="98" t="s">
-        <v>263</v>
-      </c>
-      <c r="F89" s="98"/>
-      <c r="G89" s="98"/>
-      <c r="H89" s="98"/>
-      <c r="I89" s="98"/>
-      <c r="J89" s="98"/>
-      <c r="K89" s="98"/>
-      <c r="L89" s="98"/>
-      <c r="M89" s="98"/>
+      <c r="E89" s="115" t="s">
+        <v>256</v>
+      </c>
+      <c r="F89" s="115"/>
+      <c r="G89" s="115"/>
+      <c r="H89" s="115"/>
+      <c r="I89" s="115"/>
+      <c r="J89" s="115"/>
+      <c r="K89" s="115"/>
+      <c r="L89" s="115"/>
+      <c r="M89" s="115"/>
       <c r="N89" s="3" t="s">
         <v>38</v>
       </c>
@@ -10065,7 +10057,7 @@
         <v>142</v>
       </c>
       <c r="U89" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.15">
@@ -10085,7 +10077,7 @@
       <c r="J90" s="27"/>
       <c r="K90" s="27"/>
       <c r="L90" s="27"/>
-      <c r="M90" s="104"/>
+      <c r="M90" s="88"/>
       <c r="N90" s="3" t="s">
         <v>39</v>
       </c>
@@ -10116,7 +10108,7 @@
       <c r="C91" s="10"/>
       <c r="D91" s="29"/>
       <c r="E91" s="15" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="F91" s="8"/>
       <c r="G91" s="8"/>
@@ -10148,7 +10140,7 @@
         <v>38</v>
       </c>
       <c r="U91" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.15">
@@ -10179,10 +10171,10 @@
         <v>39</v>
       </c>
       <c r="Q92" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="R92" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="S92" s="3" t="s">
         <v>39</v>
@@ -10219,10 +10211,10 @@
         <v>39</v>
       </c>
       <c r="Q93" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="R93" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="S93" s="3" t="s">
         <v>39</v>
@@ -10249,25 +10241,25 @@
       <c r="K94" s="14"/>
       <c r="L94" s="14"/>
       <c r="M94" s="50"/>
-      <c r="N94" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="O94" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="P94" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q94" s="92" t="s">
-        <v>198</v>
-      </c>
-      <c r="R94" s="92" t="s">
-        <v>198</v>
-      </c>
-      <c r="S94" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="T94" s="92" t="s">
+      <c r="N94" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="O94" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="P94" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q94" s="109" t="s">
+        <v>193</v>
+      </c>
+      <c r="R94" s="109" t="s">
+        <v>193</v>
+      </c>
+      <c r="S94" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="T94" s="109" t="s">
         <v>39</v>
       </c>
     </row>
@@ -10289,20 +10281,20 @@
       <c r="K95" s="16"/>
       <c r="L95" s="16"/>
       <c r="M95" s="13"/>
-      <c r="N95" s="93"/>
-      <c r="O95" s="93"/>
-      <c r="P95" s="93"/>
-      <c r="Q95" s="93"/>
-      <c r="R95" s="93"/>
-      <c r="S95" s="93"/>
-      <c r="T95" s="93"/>
+      <c r="N95" s="111"/>
+      <c r="O95" s="111"/>
+      <c r="P95" s="111"/>
+      <c r="Q95" s="111"/>
+      <c r="R95" s="111"/>
+      <c r="S95" s="111"/>
+      <c r="T95" s="111"/>
     </row>
     <row r="97" spans="5:14" x14ac:dyDescent="0.15">
       <c r="E97" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="N97" s="67" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="98" spans="5:14" x14ac:dyDescent="0.15">
@@ -10310,10 +10302,10 @@
         <v>119</v>
       </c>
       <c r="F98" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="N98" s="67" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="99" spans="5:14" x14ac:dyDescent="0.15">
@@ -10321,21 +10313,21 @@
         <v>38</v>
       </c>
       <c r="F99" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="N99" s="67" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="100" spans="5:14" x14ac:dyDescent="0.15">
       <c r="E100" s="37" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F100" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="N100" s="67" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="101" spans="5:14" x14ac:dyDescent="0.15">
@@ -10346,7 +10338,7 @@
         <v>134</v>
       </c>
       <c r="N101" s="67" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="102" spans="5:14" x14ac:dyDescent="0.15">
@@ -10354,19 +10346,26 @@
         <v>139</v>
       </c>
       <c r="F102" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="103" spans="5:14" x14ac:dyDescent="0.15">
       <c r="E103" s="66" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F103" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E85:M85"/>
+    <mergeCell ref="E89:M89"/>
+    <mergeCell ref="E88:M88"/>
+    <mergeCell ref="E86:M86"/>
+    <mergeCell ref="S94:S95"/>
+    <mergeCell ref="Q94:Q95"/>
+    <mergeCell ref="R94:R95"/>
     <mergeCell ref="P19:P20"/>
     <mergeCell ref="P94:P95"/>
     <mergeCell ref="A1:A2"/>
@@ -10383,13 +10382,6 @@
     <mergeCell ref="O19:O20"/>
     <mergeCell ref="T94:T95"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E85:M85"/>
-    <mergeCell ref="E89:M89"/>
-    <mergeCell ref="E88:M88"/>
-    <mergeCell ref="E86:M86"/>
-    <mergeCell ref="S94:S95"/>
-    <mergeCell ref="Q94:Q95"/>
-    <mergeCell ref="R94:R95"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -10414,37 +10406,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="86" t="s">
+      <c r="C1" s="104"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="89" t="s">
-        <v>208</v>
-      </c>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="91"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="106" t="s">
+        <v>203</v>
+      </c>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="108"/>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A2" s="85"/>
+      <c r="A2" s="102"/>
       <c r="B2" s="35" t="s">
         <v>34</v>
       </c>
@@ -10457,21 +10449,21 @@
       <c r="E2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="F2" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
       <c r="N2" s="53" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="O2" s="54" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="P2" s="35" t="s">
         <v>67</v>
@@ -10480,13 +10472,13 @@
         <v>68</v>
       </c>
       <c r="R2" s="56" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="S2" s="75" t="s">
-        <v>313</v>
-      </c>
-      <c r="T2" s="105" t="s">
-        <v>314</v>
+        <v>306</v>
+      </c>
+      <c r="T2" s="89" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.15">
@@ -10522,7 +10514,7 @@
       <c r="B4" s="10"/>
       <c r="C4" s="12"/>
       <c r="D4" s="7" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -10541,7 +10533,7 @@
       <c r="T4" s="41"/>
     </row>
     <row r="5" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="102">
+      <c r="A5" s="119">
         <v>3</v>
       </c>
       <c r="B5" s="10"/>
@@ -10558,30 +10550,30 @@
       <c r="K5" s="42"/>
       <c r="L5" s="42"/>
       <c r="M5" s="46"/>
-      <c r="N5" s="92" t="s">
-        <v>217</v>
-      </c>
-      <c r="O5" s="92" t="s">
+      <c r="N5" s="109" t="s">
+        <v>212</v>
+      </c>
+      <c r="O5" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="P5" s="92" t="s">
+      <c r="P5" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="Q5" s="92" t="s">
+      <c r="Q5" s="109" t="s">
         <v>119</v>
       </c>
-      <c r="R5" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="S5" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="T5" s="92" t="s">
+      <c r="R5" s="109" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="109" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="103"/>
+      <c r="A6" s="120"/>
       <c r="B6" s="10"/>
       <c r="C6" s="12"/>
       <c r="D6" s="26"/>
@@ -10596,16 +10588,16 @@
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
       <c r="M6" s="47"/>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
-      <c r="P6" s="93"/>
-      <c r="Q6" s="93"/>
-      <c r="R6" s="93"/>
-      <c r="S6" s="93"/>
-      <c r="T6" s="93"/>
+      <c r="N6" s="111"/>
+      <c r="O6" s="111"/>
+      <c r="P6" s="111"/>
+      <c r="Q6" s="111"/>
+      <c r="R6" s="111"/>
+      <c r="S6" s="111"/>
+      <c r="T6" s="111"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A7" s="102">
+      <c r="A7" s="119">
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
@@ -10622,38 +10614,38 @@
       <c r="K7" s="42"/>
       <c r="L7" s="42"/>
       <c r="M7" s="48"/>
-      <c r="N7" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" s="92" t="s">
+      <c r="N7" s="109" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="P7" s="92" t="s">
+      <c r="P7" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="Q7" s="92" t="s">
+      <c r="Q7" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="R7" s="92" t="s">
-        <v>204</v>
-      </c>
-      <c r="S7" s="92" t="s">
+      <c r="R7" s="109" t="s">
+        <v>199</v>
+      </c>
+      <c r="S7" s="109" t="s">
         <v>141</v>
       </c>
-      <c r="T7" s="92" t="s">
+      <c r="T7" s="109" t="s">
         <v>141</v>
       </c>
       <c r="U7" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A8" s="103"/>
+      <c r="A8" s="120"/>
       <c r="B8" s="10"/>
       <c r="C8" s="12"/>
       <c r="D8" s="26"/>
       <c r="E8" s="45" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
@@ -10663,13 +10655,13 @@
       <c r="K8" s="43"/>
       <c r="L8" s="43"/>
       <c r="M8" s="30"/>
-      <c r="N8" s="93"/>
-      <c r="O8" s="93"/>
-      <c r="P8" s="93"/>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="93"/>
-      <c r="S8" s="93"/>
-      <c r="T8" s="93"/>
+      <c r="N8" s="111"/>
+      <c r="O8" s="111"/>
+      <c r="P8" s="111"/>
+      <c r="Q8" s="111"/>
+      <c r="R8" s="111"/>
+      <c r="S8" s="111"/>
+      <c r="T8" s="111"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9" s="35">
@@ -10693,7 +10685,7 @@
         <v>38</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>38</v>
@@ -10705,7 +10697,7 @@
         <v>38</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>118</v>
@@ -10733,7 +10725,7 @@
         <v>38</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>38</v>
@@ -10758,7 +10750,7 @@
       <c r="B11" s="10"/>
       <c r="C11" s="12"/>
       <c r="D11" s="15" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="8"/>
@@ -10791,25 +10783,25 @@
         <v>118</v>
       </c>
       <c r="U11" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12" s="79"/>
       <c r="B12" s="10"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="113" t="s">
-        <v>318</v>
-      </c>
-      <c r="E12" s="114"/>
-      <c r="F12" s="115"/>
-      <c r="G12" s="115"/>
-      <c r="H12" s="115"/>
-      <c r="I12" s="115"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="115"/>
-      <c r="L12" s="115"/>
-      <c r="M12" s="115"/>
+      <c r="D12" s="97" t="s">
+        <v>310</v>
+      </c>
+      <c r="E12" s="98"/>
+      <c r="F12" s="99"/>
+      <c r="G12" s="99"/>
+      <c r="H12" s="99"/>
+      <c r="I12" s="99"/>
+      <c r="J12" s="99"/>
+      <c r="K12" s="99"/>
+      <c r="L12" s="99"/>
+      <c r="M12" s="99"/>
       <c r="N12" s="3" t="s">
         <v>38</v>
       </c>
@@ -10839,7 +10831,7 @@
       <c r="B13" s="11"/>
       <c r="C13" s="13"/>
       <c r="D13" s="15" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="8"/>
@@ -10854,10 +10846,10 @@
         <v>38</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>38</v>
@@ -10874,10 +10866,10 @@
     </row>
     <row r="22" spans="5:14" x14ac:dyDescent="0.15">
       <c r="E22" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="N22" s="67" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="5:14" x14ac:dyDescent="0.15">
@@ -10885,10 +10877,10 @@
         <v>119</v>
       </c>
       <c r="F23" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="N23" s="67" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="5:14" x14ac:dyDescent="0.15">
@@ -10896,15 +10888,15 @@
         <v>38</v>
       </c>
       <c r="F24" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="5:14" x14ac:dyDescent="0.15">
       <c r="E25" s="37" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F25" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="5:14" x14ac:dyDescent="0.15">
@@ -10920,40 +10912,40 @@
         <v>139</v>
       </c>
       <c r="F27" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="5:14" x14ac:dyDescent="0.15">
       <c r="E28" s="66" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F28" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="N1:T1"/>
-    <mergeCell ref="F2:M2"/>
     <mergeCell ref="T5:T6"/>
     <mergeCell ref="P5:P6"/>
     <mergeCell ref="Q5:Q6"/>
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="O5:O6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -10966,9 +10958,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U73"/>
+  <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -10978,37 +10970,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="86" t="s">
+      <c r="C1" s="104"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="89" t="s">
-        <v>208</v>
-      </c>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="91"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="106" t="s">
+        <v>203</v>
+      </c>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="108"/>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A2" s="85"/>
+      <c r="A2" s="102"/>
       <c r="B2" s="35" t="s">
         <v>34</v>
       </c>
@@ -11021,21 +11013,21 @@
       <c r="E2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="F2" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
       <c r="N2" s="56" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="O2" s="54" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="P2" s="35" t="s">
         <v>67</v>
@@ -11044,13 +11036,13 @@
         <v>68</v>
       </c>
       <c r="R2" s="56" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="S2" s="75" t="s">
-        <v>313</v>
-      </c>
-      <c r="T2" s="105" t="s">
-        <v>314</v>
+        <v>306</v>
+      </c>
+      <c r="T2" s="89" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.15">
@@ -11115,11 +11107,11 @@
         <v>119</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A5" s="76">
+      <c r="A5" s="85">
         <v>3</v>
       </c>
       <c r="B5" s="20"/>
@@ -11143,7 +11135,7 @@
       <c r="T5" s="39"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A6" s="76">
+      <c r="A6" s="85">
         <v>4</v>
       </c>
       <c r="B6" s="20"/>
@@ -11151,7 +11143,7 @@
       <c r="D6" s="29"/>
       <c r="E6" s="10"/>
       <c r="F6" s="7" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="8"/>
@@ -11161,7 +11153,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="8"/>
       <c r="N6" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>142</v>
@@ -11170,10 +11162,10 @@
         <v>142</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>118</v>
@@ -11183,7 +11175,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A7" s="76">
+      <c r="A7" s="85">
         <v>5</v>
       </c>
       <c r="B7" s="20"/>
@@ -11192,7 +11184,7 @@
       <c r="E7" s="10"/>
       <c r="F7" s="5"/>
       <c r="G7" s="24" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -11201,7 +11193,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="8"/>
       <c r="N7" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>142</v>
@@ -11210,10 +11202,10 @@
         <v>142</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>118</v>
@@ -11223,7 +11215,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A8" s="76">
+      <c r="A8" s="85">
         <v>6</v>
       </c>
       <c r="B8" s="20"/>
@@ -11232,7 +11224,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="24" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -11240,21 +11232,21 @@
       <c r="K8" s="8"/>
       <c r="L8" s="17"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="94" t="s">
-        <v>225</v>
-      </c>
-      <c r="O8" s="95"/>
-      <c r="P8" s="95"/>
-      <c r="Q8" s="95"/>
-      <c r="R8" s="95"/>
-      <c r="S8" s="95"/>
-      <c r="T8" s="96"/>
+      <c r="N8" s="112" t="s">
+        <v>319</v>
+      </c>
+      <c r="O8" s="113"/>
+      <c r="P8" s="113"/>
+      <c r="Q8" s="113"/>
+      <c r="R8" s="113"/>
+      <c r="S8" s="113"/>
+      <c r="T8" s="114"/>
       <c r="U8" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A9" s="76">
+      <c r="A9" s="85">
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -11280,7 +11272,7 @@
       <c r="T9" s="39"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A10" s="76">
+      <c r="A10" s="85">
         <v>8</v>
       </c>
       <c r="B10" s="20"/>
@@ -11318,7 +11310,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A11" s="76">
+      <c r="A11" s="85">
         <v>9</v>
       </c>
       <c r="B11" s="20"/>
@@ -11356,7 +11348,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A12" s="76">
+      <c r="A12" s="85">
         <v>10</v>
       </c>
       <c r="B12" s="20"/>
@@ -11394,7 +11386,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A13" s="76">
+      <c r="A13" s="85">
         <v>11</v>
       </c>
       <c r="B13" s="20"/>
@@ -11432,7 +11424,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A14" s="76">
+      <c r="A14" s="85">
         <v>12</v>
       </c>
       <c r="B14" s="20"/>
@@ -11470,7 +11462,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A15" s="76">
+      <c r="A15" s="85">
         <v>13</v>
       </c>
       <c r="B15" s="20"/>
@@ -11508,7 +11500,7 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A16" s="76">
+      <c r="A16" s="85">
         <v>14</v>
       </c>
       <c r="B16" s="20"/>
@@ -11546,7 +11538,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A17" s="76">
+      <c r="A17" s="85">
         <v>15</v>
       </c>
       <c r="B17" s="20"/>
@@ -11584,7 +11576,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A18" s="76">
+      <c r="A18" s="85">
         <v>16</v>
       </c>
       <c r="B18" s="20"/>
@@ -11622,13 +11614,13 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A19" s="76">
+      <c r="A19" s="85">
         <v>17</v>
       </c>
       <c r="B19" s="20"/>
       <c r="E19" s="5"/>
       <c r="F19" s="14" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="8"/>
@@ -11660,14 +11652,14 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A20" s="76">
+      <c r="A20" s="85">
         <v>18</v>
       </c>
       <c r="B20" s="20"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="17" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
@@ -11698,14 +11690,14 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A21" s="76">
+      <c r="A21" s="85">
         <v>19</v>
       </c>
       <c r="B21" s="20"/>
       <c r="E21" s="5"/>
       <c r="F21" s="11"/>
       <c r="G21" s="24" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
@@ -11736,12 +11728,12 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A22" s="76">
+      <c r="A22" s="85">
         <v>20</v>
       </c>
       <c r="B22" s="20"/>
       <c r="E22" s="57" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="F22" s="63"/>
       <c r="G22" s="62"/>
@@ -11774,13 +11766,13 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A23" s="76">
+      <c r="A23" s="85">
         <v>21</v>
       </c>
       <c r="B23" s="20"/>
       <c r="E23" s="82"/>
       <c r="F23" s="58" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G23" s="62"/>
       <c r="H23" s="63"/>
@@ -11812,13 +11804,13 @@
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A24" s="76">
+      <c r="A24" s="85">
         <v>22</v>
       </c>
       <c r="B24" s="20"/>
       <c r="E24" s="82"/>
       <c r="F24" s="58" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G24" s="62"/>
       <c r="H24" s="63"/>
@@ -11850,7 +11842,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A25" s="76">
+      <c r="A25" s="85">
         <v>23</v>
       </c>
       <c r="B25" s="20"/>
@@ -11890,12 +11882,12 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A26" s="76">
+      <c r="A26" s="85">
         <v>24</v>
       </c>
       <c r="B26" s="20"/>
       <c r="E26" s="7" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="17"/>
@@ -11928,13 +11920,13 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A27" s="76">
+      <c r="A27" s="85">
         <v>25</v>
       </c>
       <c r="B27" s="20"/>
       <c r="E27" s="5"/>
       <c r="F27" s="8" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="8"/>
@@ -11966,7 +11958,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A28" s="76">
+      <c r="A28" s="85">
         <v>26</v>
       </c>
       <c r="B28" s="21"/>
@@ -11974,7 +11966,7 @@
       <c r="D28" s="30"/>
       <c r="E28" s="5"/>
       <c r="F28" s="8" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="8"/>
@@ -12006,11 +11998,11 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A29" s="76">
+      <c r="A29" s="85">
         <v>27</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
@@ -12029,11 +12021,11 @@
       <c r="S29" s="38"/>
       <c r="T29" s="39"/>
       <c r="U29" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A30" s="76">
+      <c r="A30" s="85">
         <v>28</v>
       </c>
       <c r="B30" s="20"/>
@@ -12071,7 +12063,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A31" s="76">
+      <c r="A31" s="85">
         <v>29</v>
       </c>
       <c r="B31" s="26"/>
@@ -12111,7 +12103,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A32" s="76">
+      <c r="A32" s="85">
         <v>30</v>
       </c>
       <c r="B32" s="26"/>
@@ -12119,7 +12111,7 @@
       <c r="D32" s="26"/>
       <c r="E32" s="5"/>
       <c r="F32" s="7" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="8"/>
@@ -12127,17 +12119,17 @@
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="L32" s="17"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="86"/>
+      <c r="O32" s="86"/>
+      <c r="P32" s="86"/>
+      <c r="Q32" s="86"/>
+      <c r="R32" s="86"/>
+      <c r="S32" s="86"/>
+      <c r="T32" s="87"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A33" s="76">
+      <c r="A33" s="85">
         <v>31</v>
       </c>
       <c r="B33" s="26"/>
@@ -12146,7 +12138,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="17" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
@@ -12177,7 +12169,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A34" s="76">
+      <c r="A34" s="85">
         <v>32</v>
       </c>
       <c r="B34" s="26"/>
@@ -12186,7 +12178,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="6"/>
       <c r="G34" s="17" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
@@ -12217,7 +12209,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A35" s="76">
+      <c r="A35" s="85">
         <v>33</v>
       </c>
       <c r="B35" s="26"/>
@@ -12225,7 +12217,7 @@
       <c r="D35" s="26"/>
       <c r="E35" s="5"/>
       <c r="F35" s="7" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="G35" s="17"/>
       <c r="H35" s="8"/>
@@ -12233,17 +12225,17 @@
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="17"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
-      <c r="T35" s="3"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="86"/>
+      <c r="O35" s="86"/>
+      <c r="P35" s="86"/>
+      <c r="Q35" s="86"/>
+      <c r="R35" s="86"/>
+      <c r="S35" s="86"/>
+      <c r="T35" s="87"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A36" s="76">
+      <c r="A36" s="85">
         <v>34</v>
       </c>
       <c r="B36" s="26"/>
@@ -12252,7 +12244,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="17" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
@@ -12279,11 +12271,11 @@
         <v>39</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>39</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A37" s="76">
+      <c r="A37" s="85">
         <v>35</v>
       </c>
       <c r="B37" s="26"/>
@@ -12292,7 +12284,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="6"/>
       <c r="G37" s="17" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
@@ -12319,61 +12311,61 @@
         <v>39</v>
       </c>
       <c r="T37" s="3" t="s">
-        <v>39</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A38" s="76">
+      <c r="A38" s="85">
         <v>36</v>
       </c>
       <c r="B38" s="26"/>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="107" t="s">
+      <c r="F38" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="G38" s="108"/>
-      <c r="H38" s="109"/>
-      <c r="I38" s="109"/>
-      <c r="J38" s="109"/>
-      <c r="K38" s="109"/>
-      <c r="L38" s="108"/>
-      <c r="M38" s="110"/>
-      <c r="N38" s="111" t="s">
-        <v>38</v>
-      </c>
-      <c r="O38" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="P38" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q38" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="R38" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="S38" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="T38" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="U38" s="112" t="s">
-        <v>317</v>
+      <c r="G38" s="92"/>
+      <c r="H38" s="93"/>
+      <c r="I38" s="93"/>
+      <c r="J38" s="93"/>
+      <c r="K38" s="93"/>
+      <c r="L38" s="92"/>
+      <c r="M38" s="94"/>
+      <c r="N38" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="O38" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="P38" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q38" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="R38" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="S38" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="T38" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="U38" s="96" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A39" s="76">
+      <c r="A39" s="85">
         <v>37</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
       <c r="E39" s="7" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F39" s="19"/>
       <c r="G39" s="26"/>
@@ -12392,7 +12384,7 @@
       <c r="T39" s="51"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A40" s="76">
+      <c r="A40" s="85">
         <v>38</v>
       </c>
       <c r="B40" s="26"/>
@@ -12432,7 +12424,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A41" s="76">
+      <c r="A41" s="85">
         <v>39</v>
       </c>
       <c r="B41" s="26"/>
@@ -12472,7 +12464,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A42" s="76">
+      <c r="A42" s="85">
         <v>40</v>
       </c>
       <c r="B42" s="26"/>
@@ -12512,7 +12504,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A43" s="76">
+      <c r="A43" s="85">
         <v>41</v>
       </c>
       <c r="B43" s="26"/>
@@ -12552,7 +12544,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A44" s="76">
+      <c r="A44" s="85">
         <v>42</v>
       </c>
       <c r="B44" s="26"/>
@@ -12592,7 +12584,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A45" s="76">
+      <c r="A45" s="85">
         <v>43</v>
       </c>
       <c r="B45" s="26"/>
@@ -12618,7 +12610,7 @@
       <c r="T45" s="83"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A46" s="76">
+      <c r="A46" s="85">
         <v>44</v>
       </c>
       <c r="B46" s="26"/>
@@ -12626,7 +12618,7 @@
       <c r="D46" s="26"/>
       <c r="E46" s="10"/>
       <c r="F46" s="7" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="G46" s="25"/>
       <c r="H46" s="14"/>
@@ -12644,7 +12636,7 @@
       <c r="T46" s="78"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A47" s="76">
+      <c r="A47" s="85">
         <v>45</v>
       </c>
       <c r="B47" s="26"/>
@@ -12653,7 +12645,7 @@
       <c r="E47" s="10"/>
       <c r="F47" s="5"/>
       <c r="G47" s="15" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
@@ -12684,7 +12676,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A48" s="76">
+      <c r="A48" s="85">
         <v>46</v>
       </c>
       <c r="B48" s="26"/>
@@ -12724,7 +12716,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A49" s="76">
+      <c r="A49" s="85">
         <v>47</v>
       </c>
       <c r="B49" s="26"/>
@@ -12733,7 +12725,7 @@
       <c r="E49" s="10"/>
       <c r="F49" s="6"/>
       <c r="G49" s="15" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
@@ -12764,7 +12756,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A50" s="76">
+      <c r="A50" s="85">
         <v>48</v>
       </c>
       <c r="B50" s="26"/>
@@ -12772,7 +12764,7 @@
       <c r="D50" s="26"/>
       <c r="E50" s="10"/>
       <c r="F50" s="7" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="G50" s="17"/>
       <c r="H50" s="8"/>
@@ -12780,17 +12772,17 @@
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
       <c r="L50" s="17"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="86"/>
+      <c r="O50" s="86"/>
+      <c r="P50" s="86"/>
+      <c r="Q50" s="86"/>
+      <c r="R50" s="86"/>
+      <c r="S50" s="86"/>
+      <c r="T50" s="87"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A51" s="76">
+      <c r="A51" s="85">
         <v>49</v>
       </c>
       <c r="B51" s="26"/>
@@ -12799,7 +12791,7 @@
       <c r="E51" s="10"/>
       <c r="F51" s="5"/>
       <c r="G51" s="15" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
@@ -12830,7 +12822,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A52" s="76">
+      <c r="A52" s="85">
         <v>50</v>
       </c>
       <c r="B52" s="26"/>
@@ -12838,42 +12830,42 @@
       <c r="D52" s="26"/>
       <c r="E52" s="10"/>
       <c r="F52" s="6"/>
-      <c r="G52" s="107" t="s">
+      <c r="G52" s="91" t="s">
         <v>159</v>
       </c>
-      <c r="H52" s="109"/>
-      <c r="I52" s="109"/>
-      <c r="J52" s="109"/>
-      <c r="K52" s="109"/>
-      <c r="L52" s="108"/>
-      <c r="M52" s="110"/>
-      <c r="N52" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="O52" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="P52" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q52" s="111" t="s">
-        <v>38</v>
-      </c>
-      <c r="R52" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="S52" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="T52" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="U52" s="112" t="s">
-        <v>317</v>
+      <c r="H52" s="93"/>
+      <c r="I52" s="93"/>
+      <c r="J52" s="93"/>
+      <c r="K52" s="93"/>
+      <c r="L52" s="92"/>
+      <c r="M52" s="94"/>
+      <c r="N52" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="O52" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="P52" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q52" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="R52" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="S52" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="T52" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="U52" s="96" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A53" s="76">
+      <c r="A53" s="85">
         <v>51</v>
       </c>
       <c r="B53" s="26"/>
@@ -12881,7 +12873,7 @@
       <c r="D53" s="26"/>
       <c r="E53" s="10"/>
       <c r="F53" s="7" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="G53" s="17"/>
       <c r="H53" s="8"/>
@@ -12889,17 +12881,17 @@
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
       <c r="L53" s="17"/>
-      <c r="M53" s="9"/>
-      <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
-      <c r="R53" s="3"/>
-      <c r="S53" s="3"/>
-      <c r="T53" s="3"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="86"/>
+      <c r="O53" s="86"/>
+      <c r="P53" s="86"/>
+      <c r="Q53" s="86"/>
+      <c r="R53" s="86"/>
+      <c r="S53" s="86"/>
+      <c r="T53" s="87"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A54" s="76">
+      <c r="A54" s="85">
         <v>52</v>
       </c>
       <c r="B54" s="26"/>
@@ -12907,42 +12899,42 @@
       <c r="D54" s="26"/>
       <c r="E54" s="10"/>
       <c r="F54" s="5"/>
-      <c r="G54" s="107" t="s">
-        <v>187</v>
-      </c>
-      <c r="H54" s="108"/>
-      <c r="I54" s="109"/>
-      <c r="J54" s="109"/>
-      <c r="K54" s="109"/>
-      <c r="L54" s="108"/>
-      <c r="M54" s="110"/>
-      <c r="N54" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="O54" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="P54" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q54" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="R54" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="S54" s="111" t="s">
-        <v>38</v>
-      </c>
-      <c r="T54" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="U54" s="112" t="s">
-        <v>317</v>
+      <c r="G54" s="91" t="s">
+        <v>182</v>
+      </c>
+      <c r="H54" s="92"/>
+      <c r="I54" s="93"/>
+      <c r="J54" s="93"/>
+      <c r="K54" s="93"/>
+      <c r="L54" s="92"/>
+      <c r="M54" s="94"/>
+      <c r="N54" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="O54" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="P54" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q54" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="R54" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="S54" s="95" t="s">
+        <v>119</v>
+      </c>
+      <c r="T54" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="U54" s="96" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A55" s="76">
+      <c r="A55" s="85">
         <v>53</v>
       </c>
       <c r="B55" s="26"/>
@@ -12951,7 +12943,7 @@
       <c r="E55" s="10"/>
       <c r="F55" s="5"/>
       <c r="G55" s="15" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="H55" s="17"/>
       <c r="I55" s="8"/>
@@ -12975,14 +12967,14 @@
         <v>39</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="T55" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A56" s="76">
+      <c r="A56" s="85">
         <v>54</v>
       </c>
       <c r="B56" s="26"/>
@@ -12991,7 +12983,7 @@
       <c r="E56" s="10"/>
       <c r="F56" s="6"/>
       <c r="G56" s="15" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H56" s="17"/>
       <c r="I56" s="8"/>
@@ -13022,14 +13014,14 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A57" s="76">
+      <c r="A57" s="85">
         <v>55</v>
       </c>
       <c r="B57" s="26"/>
       <c r="C57" s="26"/>
       <c r="D57" s="26"/>
       <c r="E57" s="57" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F57" s="58"/>
       <c r="G57" s="59"/>
@@ -13048,7 +13040,7 @@
       <c r="T57" s="52"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A58" s="76">
+      <c r="A58" s="85">
         <v>56</v>
       </c>
       <c r="B58" s="26"/>
@@ -13056,7 +13048,7 @@
       <c r="D58" s="26"/>
       <c r="E58" s="60"/>
       <c r="F58" s="61" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G58" s="62"/>
       <c r="H58" s="63"/>
@@ -13069,7 +13061,7 @@
         <v>39</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>186</v>
+        <v>119</v>
       </c>
       <c r="P58" s="3" t="s">
         <v>39</v>
@@ -13088,7 +13080,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A59" s="76">
+      <c r="A59" s="85">
         <v>57</v>
       </c>
       <c r="B59" s="26"/>
@@ -13096,7 +13088,7 @@
       <c r="D59" s="26"/>
       <c r="E59" s="60"/>
       <c r="F59" s="61" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G59" s="62"/>
       <c r="H59" s="63"/>
@@ -13109,7 +13101,7 @@
         <v>39</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>183</v>
+        <v>119</v>
       </c>
       <c r="P59" s="3" t="s">
         <v>39</v>
@@ -13128,7 +13120,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A60" s="76">
+      <c r="A60" s="85">
         <v>58</v>
       </c>
       <c r="B60" s="26"/>
@@ -13136,7 +13128,7 @@
       <c r="D60" s="26"/>
       <c r="E60" s="60"/>
       <c r="F60" s="61" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="G60" s="62"/>
       <c r="H60" s="63"/>
@@ -13149,7 +13141,7 @@
         <v>39</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>183</v>
+        <v>119</v>
       </c>
       <c r="P60" s="3" t="s">
         <v>39</v>
@@ -13168,16 +13160,16 @@
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A61" s="76">
+      <c r="A61" s="85">
         <v>59</v>
       </c>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="57" t="s">
-        <v>268</v>
-      </c>
-      <c r="F61" s="58"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="61" t="s">
+        <v>261</v>
+      </c>
+      <c r="F61" s="63"/>
       <c r="G61" s="62"/>
       <c r="H61" s="63"/>
       <c r="I61" s="63"/>
@@ -13186,7 +13178,7 @@
       <c r="L61" s="62"/>
       <c r="M61" s="64"/>
       <c r="N61" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O61" s="3" t="s">
         <v>39</v>
@@ -13198,7 +13190,7 @@
         <v>39</v>
       </c>
       <c r="R61" s="3" t="s">
-        <v>38</v>
+        <v>213</v>
       </c>
       <c r="S61" s="3" t="s">
         <v>38</v>
@@ -13207,212 +13199,66 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A62" s="76">
-        <v>60</v>
-      </c>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F62" s="8"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="19"/>
-      <c r="I62" s="19"/>
-      <c r="J62" s="19"/>
-      <c r="K62" s="19"/>
-      <c r="L62" s="26"/>
-      <c r="M62" s="8"/>
-      <c r="N62" s="38"/>
-      <c r="O62" s="38"/>
-      <c r="P62" s="38"/>
-      <c r="Q62" s="38"/>
-      <c r="R62" s="38"/>
-      <c r="S62" s="38"/>
-      <c r="T62" s="39"/>
-    </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A63" s="76">
-        <v>61</v>
-      </c>
-      <c r="B63" s="26"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="G63" s="17"/>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
-      <c r="J63" s="8"/>
-      <c r="K63" s="8"/>
-      <c r="L63" s="17"/>
-      <c r="M63" s="9"/>
-      <c r="N63" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O63" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P63" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q63" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R63" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S63" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T63" s="3" t="s">
-        <v>39</v>
+      <c r="E63" t="s">
+        <v>194</v>
+      </c>
+      <c r="N63" s="67" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A64" s="76">
-        <v>62</v>
-      </c>
-      <c r="B64" s="26"/>
-      <c r="C64" s="26"/>
-      <c r="D64" s="26"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="G64" s="17"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
-      <c r="K64" s="8"/>
-      <c r="L64" s="17"/>
-      <c r="M64" s="9"/>
-      <c r="N64" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O64" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P64" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q64" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R64" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S64" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T64" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A65" s="76">
-        <v>63</v>
-      </c>
-      <c r="B65" s="21"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="G65" s="23"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
-      <c r="J65" s="16"/>
-      <c r="K65" s="16"/>
-      <c r="L65" s="23"/>
-      <c r="M65" s="13"/>
-      <c r="N65" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O65" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P65" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q65" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R65" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S65" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T65" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E67" t="s">
-        <v>199</v>
-      </c>
-      <c r="N67" s="67" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="E64" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="F64" t="s">
+        <v>198</v>
+      </c>
+      <c r="N64" s="67" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="65" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E65" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F65" t="s">
+        <v>195</v>
+      </c>
+      <c r="N65" s="74" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="66" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E66" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="F66" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="67" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E67" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="F67" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="5:14" x14ac:dyDescent="0.15">
       <c r="E68" s="37" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="F68" t="s">
-        <v>203</v>
-      </c>
-      <c r="N68" s="67" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E69" s="37" t="s">
-        <v>38</v>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="69" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E69" s="66" t="s">
+        <v>200</v>
       </c>
       <c r="F69" t="s">
-        <v>200</v>
-      </c>
-      <c r="N69" s="74" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E70" s="37" t="s">
-        <v>202</v>
-      </c>
-      <c r="F70" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E71" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="F71" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E72" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="F72" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E73" s="66" t="s">
-        <v>205</v>
-      </c>
-      <c r="F73" t="s">
-        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>